<commit_message>
Build XML mostly working Can't handle spaces in TemplateID Progress Bar not working
</commit_message>
<xml_diff>
--- a/GUI_Management/Options and Functions.xlsx
+++ b/GUI_Management/Options and Functions.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greg\OneDrive - Queen's University\Python\Projects\EclipseRelated\EclipseTemplates\ManageStructuresTemplates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="12030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="12030" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pack and Grid Methods" sheetId="1" r:id="rId1"/>
+    <sheet name="Pack and Grid Methods (2)" sheetId="2" r:id="rId2"/>
+    <sheet name="TTK Options" sheetId="3" r:id="rId3"/>
+    <sheet name="Widgets" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'TTK Options'!$A$1:$C$163</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="321">
   <si>
     <t>Layout Method</t>
   </si>
@@ -249,13 +250,1261 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Function Calls</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the widget has an associated horizontal scrollbar, set this option to the .set method of that scrollbar. </t>
+  </si>
+  <si>
+    <r>
+      <t>xscrollcommand</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Entry</t>
+  </si>
+  <si>
+    <t>Combobox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you set this option to some dimension, all the text will be chopped into lines no longer than this dimension. This option may also be specified through a style. </t>
+  </si>
+  <si>
+    <r>
+      <t>wraplength</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option to specify a fixed width or a minimum width. The value is specified in characters; a positive value sets a fixed width of that many average characters, while a negative width sets a minimum width. 
+You may also specify a width value in an associated style. If values are specified both in the widget constructor call and in the style, the former takes priority. </t>
+  </si>
+  <si>
+    <r>
+      <t>width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Radiobutton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The width dimension of the widget. </t>
+  </si>
+  <si>
+    <t>PanedWindow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The width in pixels to be allocated to the widget. </t>
+  </si>
+  <si>
+    <t>Notebook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the label is text, this option specifies the absolute width of the text area on the button, as a number of characters; the actual width is that number multiplied by the average width of a character in the current font. For image labels, this option is ignored. The option may also be configured in a style. </t>
+  </si>
+  <si>
+    <t>Menubutton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This option can be set to some dimension to specify the width of the frame. If you don't call the .grid_propagate(0) method, this option will be ignored; see Section 4.2, “Other grid management methods”. </t>
+  </si>
+  <si>
+    <t>LabelFrame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To specify a fixed width, set this option to the number of characters. To specify a minimum width, set this option to minus the number of characters. If you don't specify this option, the size of the label area will be just enough to accommodate the current text and/or image. 
+For text displayed in a proportional font, the actual width of the widget will be based on the average width of a character in the font, and not a specific number of characters. 
+This option may also be specified through a style. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This option is a dimension that sets the width of the frame. If you want to force the frame to have a specific width, call the .grid_propagate(0) on the widget; see Section 4.2, “Other grid management methods”. </t>
+  </si>
+  <si>
+    <t>Frame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This option specifies the width of the entry area as a number of characters. The actual width will be this number times the average width of a character in the effective font. The default value is 20. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option to specify a fixed width or a minimum width. The value is specified in characters; a positive value sets a fixed width of that many average characters, while a negative width sets a minimum width. 
+For example, if an average character in the selected font is 10 pixels wide, option width=8 will make the text label exactly 80 pixels wide; option width=-8 will use 80 pixels or the length of the text, whichever is larger. 
+You may also specify a width value in an associated style. If values are specified both in the widget constructor call and in the style, the former takes priority. 
+</t>
+  </si>
+  <si>
+    <t>Checkbutton</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option to associate a control variable with the widget. Typically this will be a tk.DoubleVar instance, which holds a value of type float. You may instead use a tk.IntVar instance, but values stored in it will be truncated as type int. </t>
+  </si>
+  <si>
+    <r>
+      <t>variable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A control variable that is shared by the other radiobuttons in the group; see Section 52, “Control variables: the values behind the widgets”. The type of this variable will be the same as the type you specify for the value options for the radiobuttons in the group. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option to link a control variable to the widget so that you can get or set the current value of the indicator. </t>
+  </si>
+  <si>
+    <t>Progressbar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A control variable that tracks the current state of the checkbutton; see Section 52, “Control variables: the values behind the widgets”. Normally you will use an IntVar here, and the off and on values are 0 and 1, respectively. However, you may use a different control variable type, and specify the offvalue and onvalue options using values of that type. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The choices that will appear in the drop-down menu, as a sequence of strings. </t>
+  </si>
+  <si>
+    <r>
+      <t>values</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option to set the initial value of the widget's variable; the default is 0.0. </t>
+  </si>
+  <si>
+    <r>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The value associated with this radiobutton. When the radiobutton is the one selected in the group, the value of this option will be stored in the control variable for the group. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">See Section 10.2, “Adding validation to an Entry widget”. </t>
+  </si>
+  <si>
+    <r>
+      <t>validatecommand</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">You may use this option to specify a callback function that dynamically validates the widget's text content. See Section 10.2, “Adding validation to an Entry widget”. </t>
+  </si>
+  <si>
+    <r>
+      <t>validate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">You may use this option to request dynamic validation of the widget's text content. See Section 10.2, “Adding validation to an Entry widget”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If this option has a nonnegative value n, an underline will appear under the text character at position n. </t>
+  </si>
+  <si>
+    <r>
+      <t>underline</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">If this option has a nonnegative value n, an underline will appear under the character at position n. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can request that one of the letters in the text string be underline by setting this option to the position of that letter. For example, if you specified text='Panic' and underline=2, an underline would appear under the 'n'. 
+Using this option doesn't change anything functionally. If you want the application to react to the Q key or some variation like control-shift-Q, you'll need to set up the bindings using the event system. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can request that one of the letters in the text string be underline by setting this option to the position of that letter. For example, the options text='Quit' and underline=0 would underline the Q. 
+Using this option doesn't change anything functionally. If you want the application to react to the Q key or some variation like control-shift-Q, you'll need to set up the bindings using the event system. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A float value that defines one end of the scale's range; the other end is defined by the from_ option, discussed above. The to value can be either greater than or less than the from_ value. For vertical scales, the to value defines the bottom of the scale; for horizontal scales, the right end. The default value is 100. </t>
+  </si>
+  <si>
+    <r>
+      <t>to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">A variable that controls the text that appears on the radiobutton; see Section 52, “Control variables: the values behind the widgets”. </t>
+  </si>
+  <si>
+    <r>
+      <t>textvariable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">A variable that controls the text that appears on the menubutton; see Section 52, “Control variables: the values behind the widgets”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A StringVar instance (see Section 52, “Control variables: the values behind the widgets”); the text displayed on the widget will be its value. If both text and textvariable are specified, the text option will be ignored. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A variable that controls the text that appears in the entry area; see Section 52, “Control variables: the values behind the widgets”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A variable that controls the text that appears on the checkbutton; see Section 52, “Control variables: the values behind the widgets”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A variable that controls the text that appears on the button; see Section 52, “Control variables: the values behind the widgets”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The text to appear next to the radiobutton, as a string. </t>
+  </si>
+  <si>
+    <r>
+      <t>text</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The text to appear on the menubutton, as a string. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The value of this option is a string that will appear as part of the border. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A string of text to be displayed in the widget. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The text to appear on the checkbutton, as a string. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The text to appear on the button, as a string. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">By default, a ttk.Scrollbar will not be included in focus traversal; see Section 53, “Focus: routing keyboard input”. To add the widget to focus traversal, use takefocus=True. </t>
+  </si>
+  <si>
+    <r>
+      <t>takefocus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Scrollbar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">By default, a ttk.Scale widget will be included in focus traversal; see Section 53, “Focus: routing keyboard input”. To remove the widget from focus traversal, use takefocus=False. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">By default, a ttk.Radiobutton will be included in focus traversal; see Section 53, “Focus: routing keyboard input”. To remove the widget from focus traversal, use takefocus=False. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">By default, a ttk.Progressbar will not be included in focus traversal; see Section 53, “Focus: routing keyboard input”. To add the widget to focus traversal, use takefocus=True. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">By default, a ttk.PanedWindow will not be included in focus traversal; see Section 53, “Focus: routing keyboard input”. To add the widget to focus traversal, use takefocus=True. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">By default, a ttk.Notebook will be included in focus traversal; see Section 53, “Focus: routing keyboard input”. To remove the widget from focus traversal, use takefocus=False. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">By default, a ttk.Menubutton will be included in focus traversal; see Section 53, “Focus: routing keyboard input”. To remove the widget from focus traversal, use takefocus=False. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option to specify whether the widget is visited during focus traversal; see Section 53, “Focus: routing keyboard input”. Specify takefocus=True if you want the visit to accept focus; specify takefocus=False if the widget is not to accept focus. 
+The default value is an empty string; by default, ttk.Label widgets do not get focus. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option to specify whether the widget is visited during focus traversal; see Section 53, “Focus: routing keyboard input”. Specify takefocus=True if you want the visit to accept focus; specify takefocus=False if the widget is not to accept focus. 
+The default value is an empty string; by default, ttk.Label widgets do not get focus. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option to specify whether a widget is visited during focus traversal; see Section 53, “Focus: routing keyboard input”. Specify takefocus=True if you want the visit to accept focus; specify takefocus=False if the widget is not to accept focus. The default value is an empty string; by default, ttk.Frame widgets do not get focus. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">By default, a ttk.Checkbutton will be included in focus traversal; see Section 53, “Focus: routing keyboard input”. To remove the widget from focus traversal, use takefocus=False. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">By default, a ttk.Button will be included in focus traversal; see Section 53, “Focus: routing keyboard input”. To remove the widget from focus traversal, use takefocus=False. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The style to be used in rendering this scrollbar; see Section 49, “Using and customizing ttk styles”. The only style feature you can configure is background, which specifies the color of the separator bar; the default color is a dark gray. </t>
+  </si>
+  <si>
+    <r>
+      <t>style</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Separator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The style to be used in rendering this scrollbar; see Section 49, “Using and customizing ttk styles”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The style to be used in rendering this radiobutton; see Section 49, “Using and customizing ttk styles”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The style to be used in rendering this widget; see Section 49, “Using and customizing ttk styles”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The style to be used in rendering this menubutton; see Section 49, “Using and customizing ttk styles”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option to specify a custom widget style name; see Section 47, “Customizing and creating ttk themes and styles”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The style to be used in rendering this checkbutton; see Section 49, “Using and customizing ttk styles”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The style to be used in rendering this button; see Section 49, “Using and customizing ttk styles”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To protect fields such as passwords from being visible on the screen, set this option to a string, whose first character will be substituted for each of the actual characters in the field. For example, if the field contains “ sesame” but you have specified show='*', the field will appear as “******”. </t>
+  </si>
+  <si>
+    <r>
+      <t>show</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option to specify a 3-d border style; see Section 5.6, “Relief styles”. You will need to specify a nonzero borderwidth for this effect to appear. This option may also be specified by a style. </t>
+  </si>
+  <si>
+    <r>
+      <t>relief</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Set this option to a relief style to create a 3-d effect. You will need to increase the borderwidth to make this effect appear. You may also specify this option using a style. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specifies the relief style for the border; see Section 5.6, “Relief styles”. This has no effect unless you also increase the borderwidth. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You may use this option to supply a callback function that will be invoked when the user clicks on the down-arrow. This callback may change the values option; if so, the changes will appear in the drop-down menu. </t>
+  </si>
+  <si>
+    <r>
+      <t>postcommand</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">To add some extra space around the outside of the widget, set this option to that amount of space as a dimension. </t>
+  </si>
+  <si>
+    <r>
+      <t>padding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">To add extra clear area around the contents of this widget, set this option to a dimension. This option may also be specified by a style. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To add more space around all four sides of the text and/or image, set this option to the desired dimension. You may also specify this option using a style. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To create an empty area inside the frame and outside of the contained widgets, set this option to the desired dimension. For example, padding='0.5i' would clear a half-inch-wide area inside the frame and around the outside of the widgets inside it. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set orient=tk.HORIZONTAL for a horizontal separator, orient=tk.VERTICAL for a vertical one (the default orientation). </t>
+  </si>
+  <si>
+    <r>
+      <t>orient</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Set orient=tk.HORIZONTAL for a horizontal scrollbar, orient=tk.VERTICAL for a vertical one (the default orientation). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set orient=tk.HORIZONTAL if you want the scale to run along the x dimension, or orient=tk.VERTICAL to run parallel to the y-axis. Default is vertical. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This options specifies the orientation: use orient=tk.HORIZONTAL or orient=tk.VERTICAL. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To stack child widgets side by side, use orient=tk.HORIZONTAL. To stack them top to bottom, use orient=tk.VERTICAL. The default option is tk.VERTICAL. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">By default, when a checkbutton is in the on (checked) state, the value of the associated variable is 1. You can use the onvalue option to specify a different value for the on state. </t>
+  </si>
+  <si>
+    <r>
+      <t>onvalue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">By default, when a checkbutton is in the off (unchecked) state, the value of the associated variable is 0. You can use the offvalue option to specify a different value for the off state. </t>
+  </si>
+  <si>
+    <r>
+      <t>offvalue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">If your program cannot accurately depict the relative progress that this widget is supposed to display, use mode='indeterminate'. In this mode, a rectangle bounces back and forth between the ends of the widget once you use the .start() method. 
+If your program has some measure of relative progress, use mode='determinate'. In this mode, your program can move the indicator to a specified position along the widget's track. </t>
+  </si>
+  <si>
+    <r>
+      <t>mode</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The related Menu widget. See Section 15, “The Menu widget” for the procedure used to establish this mutual connection. </t>
+  </si>
+  <si>
+    <r>
+      <t>menu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum value of the indicator; default is 100. </t>
+  </si>
+  <si>
+    <r>
+      <t>maximum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The length of the scale widget. This is the x dimension if the scale is horizontal, or the y dimension if vertical. The default is 100 pixels. For allowable values, see Section 5.1, “Dimensions”. </t>
+  </si>
+  <si>
+    <r>
+      <t>length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The size of the widget along its long axis as a dimension. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instead of a text label, you can use any widget as the label in a ttk.LabelFrame. Create some widget w but do not register it with the .grid() method. Then create the LabelFrame with labelwidget=w. If you specify this option as well as the text option, the latter is ignored. 
+For example, if you don't like the rather small and plain default font used for the label, you can use this option to display a Label widget with the font and other appearance of your choice. </t>
+  </si>
+  <si>
+    <r>
+      <t>labelwidget</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option to specify the position of the label on the widget's border. The default position is 'nw', which places the label at the left end of the top border. For the nine possible label positions, refer to Section 13, “The LabelFrame widget”. </t>
+  </si>
+  <si>
+    <r>
+      <t>labelanchor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">If the text you provide contains newline ('\n') characters, this option specifies how each line will be positioned horizontally: tk.LEFT to left-justify; tk.CENTER to center; or tk.RIGHT to right-justify each line. You may also specify this option using a style. </t>
+  </si>
+  <si>
+    <r>
+      <t>justify</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">This option specifies how the text will be positioned within the entry area when it does not completely fill the area. Values may be tk.LEFT to left-justify; tk.CENTER to center; or tk.RIGHT to right-justify. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You may set this option to a callback function that will be called whenever validation fails (that is, when the validatecommand returns a 0). See Section 10.2, “Adding validation to an Entry widget”. </t>
+  </si>
+  <si>
+    <r>
+      <t>invalidcommand</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">An image to appear on the radiobutton; see Section 5.9, “Images”. </t>
+  </si>
+  <si>
+    <r>
+      <t>image</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">An image to appear on the menubutton; see Section 5.9, “Images”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This option specifies an image or images to be displayed either in addition to or instead of text. The value must be an image as specified in Section 5.9, “Images”. See the compound option above for what happens when you supply both image and text. 
+You may specify multiple images that will appear on the widget depending on the state of the widget (see Section 50.2, “ttk style maps: dynamic appearance changes” for a discussion of widget states). To do this, supply as the value of this option a tuple (i0, s1, i1, s2, i2, ...), where: 
+i0 is the default image to be displayed on the widget. 
+For each pair of values after the first, si specifies a state or combination of states, and i1 specifies the image to be displayed when the widget's state matches si. 
+Each state specifier si may be a single state name, optionally preceded by '!', or a sequence of such names. The ! specifies that the widget must not be in that state. 
+For example, suppose you have three PhotoImage instances named im1, im2, and im3, and in your call to the Label constructor you include this option: 
+    self.w = ttk.Label(self, ...,
+         image=(im1,
+                'selected', im2,
+                ('!disabled', 'alternate'), im3), ...)
+The widget will display image im2 if it is in the selected state. If it is not in the selected state or the disabled state but it is in the alternate state, it will display image im3. Otherwise it will display image im1. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">An image to appear on the checkbutton; see Section 5.9, “Images”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">An image to appear on the button; see Section 5.9, “Images”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The height dimension of the widget. </t>
+  </si>
+  <si>
+    <r>
+      <t>height</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The height in pixels to be allocated to the widget. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This option can be set to some dimension to specify the height of the frame. If you don't call the .grid_propagate(0) method, this option will be ignored; see Section 4.2, “Other grid management methods”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This option is a dimension that sets the height of the frame. If you want to force the frame to have a specific height, call the .grid_propagate(0) on the widget; see Section 4.2, “Other grid management methods”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option to specify a maximum number of rows that will appear in the drop-down menu; the default is 20. If there are more values than this number, the drop-down menu will automatically include a vertical scrollbar. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option in combination with the to option (described below) to constrain the values to a numeric range. For example, from_=-10 and to=10 would allow only values between −10 and 20 inclusive. See also the increment option below. </t>
+  </si>
+  <si>
+    <r>
+      <t>from_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option to specify the color of the displayed text. You may also specify this option using a style. </t>
+  </si>
+  <si>
+    <r>
+      <t>foreground</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option to specify the font style for the displayed text. You may also specify this option using a style. </t>
+  </si>
+  <si>
+    <r>
+      <t>font</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option to specify the font of the text that will appear in the widget; see Section 5.4, “Type fonts”. For reasons that are unclear to the author, this option cannot be specified with a style. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">By default, if you select text within an Entry widget, it is automatically exported to the clipboard. To avoid this exportation, use exportselection=0. </t>
+  </si>
+  <si>
+    <r>
+      <t>exportselection</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">This option specifies the position where the drop-down menu appears, relative to the menubutton. 
+above  The menu will appear just above the menubutton. 
+below  The menu will appear just below the menubutton. 
+flush  The menu will appear over the menubutton, so that the menu's northwest corner coincides with the menubutton's northwest corner. 
+left  The menu will appear just to the left of the menubutton. 
+right  The menu will appear just to the right of the menubutton. </t>
+  </si>
+  <si>
+    <r>
+      <t>direction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The cursor that will appear when the mouse is over the scrollbar; see Section 5.8, “Cursors”. </t>
+  </si>
+  <si>
+    <r>
+      <t>cursor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The cursor that will appear when the mouse is over the scale; see Section 5.8, “Cursors”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cursor that will appear when the mouse is over the radiobutton; see Section 5.8, “Cursors”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cursor that will appear when the mouse is over the checkbutton; see Section 5.8, “Cursors”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cursor that will appear when the mouse is over the notebook; see Section 5.8, “Cursors”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cursor that will appear when the mouse is over the button; see Section 5.8, “Cursors”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option to specify the appearance of the mouse cursor when it is over the widget; see Section 5.8, “Cursors”. The default value (an empty string) specifies that the cursor is inherited from the parent widget. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This option specifies the relative position of the image relative to the text when you specify both. The value may be tk.TOP (image above text), tk.BOTTOM (image below text), tk.LEFT (image to the left of the text), or tk.RIGHT (image to the right of the text). If you provide both image and text options but do not specify a value for compound, only the image will appear. </t>
+  </si>
+  <si>
+    <r>
+      <t>compound</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">If you provide both image and text options, the compound option specifies the position of the image relative to the text. The value may be tk.TOP (image above text), tk.BOTTOM (image below text), tk.LEFT (image to the left of the text), or tk.RIGHT (image to the right of the text). 
+When you provide both image and text options but don't specify a compound option, the image will appear and the text will not. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you provide both text and image options, the compound option specifies how to display them. 
+'bottom'  Display the image below the text. 
+'image'  Display only the image, not the text. 
+'left'  Display the image to the left of the text. 
+'none'  Display the image if there is one, otherwise display the text. This is the default value
+'right'  Display the image to the right of the text. 
+'text'  Display the text, not the image. 
+'top'  Display the image above the text.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A procedure to be called whenever the scrollbar is moved. For a discussion of the calling sequence, see Section 22.1, “The Scrollbar command callback”. </t>
+  </si>
+  <si>
+    <r>
+      <t>command</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">A function to be called whenever the state of this widget changes. This function will receive one argument, the new value shown on the widget, as a float. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A function to be called whenever the state of this radiobutton changes. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A function to be called whenever the state of this checkbutton changes. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A function to be called when the button is pressed. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The widget class name. This may be specified when the widget is created, but cannot be changed later. For an explanation of widget classes, see Section 27, “Standardizing appearance”. </t>
+  </si>
+  <si>
+    <r>
+      <t>class_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">You may provide a widget class name when you create this widget. This name may be used to customize the widget's appearance; see Section 27, “Standardizing appearance”. Once the widget is created, the widget class name cannot be changed. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option to set the width of the border around the widget to a given dimension. This option may also be configured using a style. </t>
+  </si>
+  <si>
+    <r>
+      <t>borderwidth</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">To add a border around the label, set this option to the width dimension. You may also specify this option using a style. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option to specify the width of the border element; the default is zero. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this option to set the background color. You may also specify this option using a style. </t>
+  </si>
+  <si>
+    <r>
+      <t>background</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">If the text and/or image are smaller than the specified width, you can use the anchor option to specify where to position them: tk.W, tk.CENTER, or tk.E for left, centered, or right alignment, respectively. You may also specify this option using a style. </t>
+  </si>
+  <si>
+    <r>
+      <t>anchor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Widget</t>
+  </si>
+  <si>
+    <t>Allow user to pick a file from the file system</t>
+  </si>
+  <si>
+    <t>Filedialog</t>
+  </si>
+  <si>
+    <t>Visual color picker</t>
+  </si>
+  <si>
+    <t>Colorchooser</t>
+  </si>
+  <si>
+    <t>Show pop-up with text and error icon.</t>
+  </si>
+  <si>
+    <t>showerror</t>
+  </si>
+  <si>
+    <t>Show pop-up with text and warning icon.</t>
+  </si>
+  <si>
+    <t>showwarning</t>
+  </si>
+  <si>
+    <t>Show pop-up with text and info icon.</t>
+  </si>
+  <si>
+    <t>showinfo</t>
+  </si>
+  <si>
+    <t>Ask retry or cancel</t>
+  </si>
+  <si>
+    <t>askretrycancel</t>
+  </si>
+  <si>
+    <t>Ask ok or cancel.</t>
+  </si>
+  <si>
+    <t>askokcancel</t>
+  </si>
+  <si>
+    <t>Ask yes, no, or cancel.</t>
+  </si>
+  <si>
+    <t>askyesnocancel</t>
+  </si>
+  <si>
+    <t>Ask yes or no.</t>
+  </si>
+  <si>
+    <t>askyesno</t>
+  </si>
+  <si>
+    <t>Ask a question with a yes or no response.</t>
+  </si>
+  <si>
+    <t>askquestion</t>
+  </si>
+  <si>
+    <t>Pop-up Dialog Windows</t>
+  </si>
+  <si>
+    <t>Similar to Combobox or HTML select. A dropdown option select menu.</t>
+  </si>
+  <si>
+    <t>Optionmenu</t>
+  </si>
+  <si>
+    <t>Menu bar for the top of the window. Typically things like "File", "Edit", and "View".</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>tk only</t>
+  </si>
+  <si>
+    <t>MessageBox</t>
+  </si>
+  <si>
+    <t>For drawing graphics like lines, circles, arcs, ovals, and rectangles</t>
+  </si>
+  <si>
+    <t>Canvas</t>
+  </si>
+  <si>
+    <t>A window just like the main window with its own title bar and can be moved and resized on its own. If the main window is destroyed, all other top levels are destroyed too</t>
+  </si>
+  <si>
+    <t>Toplevel</t>
+  </si>
+  <si>
+    <t>Multiple line display text that can be styled</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Multiple line select list</t>
+  </si>
+  <si>
+    <t>Listbox</t>
+  </si>
+  <si>
+    <t>Like a single line text entry widget with up and down arrows on the side to increment or decrement. Mousewheel up and down to raise and lower values</t>
+  </si>
+  <si>
+    <t>Spinbox</t>
+  </si>
+  <si>
+    <t>Multiple line editable text entry</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>ttk only</t>
+  </si>
+  <si>
+    <t>Treeview</t>
+  </si>
+  <si>
+    <t>Visually separate widgets vertically or horizontally</t>
+  </si>
+  <si>
+    <t>For adding a triangle in the bottom right corner of a window to make it easier to grab and resize</t>
+  </si>
+  <si>
+    <t>Sizegrip</t>
+  </si>
+  <si>
+    <t>Progress bars that can be customized in many ways</t>
+  </si>
+  <si>
+    <t>Tabbed contents</t>
+  </si>
+  <si>
+    <t>A single line text entry field that also has a drop down select list. Choose pre-defined items or enter a custom value.</t>
+  </si>
+  <si>
+    <t>ComboBox</t>
+  </si>
+  <si>
+    <t>Vertical or horizontal</t>
+  </si>
+  <si>
+    <t>ttk and tk</t>
+  </si>
+  <si>
+    <t>Like a frame that contains a horizontal or vertical set of frames that are resizeable in relation to each other</t>
+  </si>
+  <si>
+    <t>PannedWindow</t>
+  </si>
+  <si>
+    <t>Used as a container to house other widgets and add borders</t>
+  </si>
+  <si>
+    <t>A frame that by default displays a border and title</t>
+  </si>
+  <si>
+    <t>Labelframe</t>
+  </si>
+  <si>
+    <t>Display text or images</t>
+  </si>
+  <si>
+    <t>Lable</t>
+  </si>
+  <si>
+    <t>Sliding scale to be clicked and dragged with mouse</t>
+  </si>
+  <si>
+    <t>Standard radio buttons</t>
+  </si>
+  <si>
+    <t>Single line editable text entry</t>
+  </si>
+  <si>
+    <t>Check box for toggling a value (can have callback on click)</t>
+  </si>
+  <si>
+    <t>Standard button that calls a function when clicked</t>
+  </si>
+  <si>
+    <t>Source</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,6 +1519,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -578,7 +1833,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -588,7 +1843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -1126,4 +2381,2634 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="118.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C163"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="137.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" t="s">
+        <v>250</v>
+      </c>
+      <c r="C6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" t="s">
+        <v>247</v>
+      </c>
+      <c r="C7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" t="s">
+        <v>247</v>
+      </c>
+      <c r="C8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C9" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" t="s">
+        <v>247</v>
+      </c>
+      <c r="C10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" t="s">
+        <v>247</v>
+      </c>
+      <c r="C11" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
+        <v>247</v>
+      </c>
+      <c r="C12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" t="s">
+        <v>247</v>
+      </c>
+      <c r="C13" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" t="s">
+        <v>247</v>
+      </c>
+      <c r="C14" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
+        <v>247</v>
+      </c>
+      <c r="C15" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" t="s">
+        <v>247</v>
+      </c>
+      <c r="C16" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" t="s">
+        <v>247</v>
+      </c>
+      <c r="C17" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" t="s">
+        <v>247</v>
+      </c>
+      <c r="C18" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" t="s">
+        <v>247</v>
+      </c>
+      <c r="C19" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" t="s">
+        <v>247</v>
+      </c>
+      <c r="C20" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>156</v>
+      </c>
+      <c r="B21" t="s">
+        <v>247</v>
+      </c>
+      <c r="C21" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" t="s">
+        <v>241</v>
+      </c>
+      <c r="C22" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" t="s">
+        <v>241</v>
+      </c>
+      <c r="C23" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" t="s">
+        <v>241</v>
+      </c>
+      <c r="C24" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" t="s">
+        <v>241</v>
+      </c>
+      <c r="C25" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>142</v>
+      </c>
+      <c r="B26" t="s">
+        <v>241</v>
+      </c>
+      <c r="C26" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" t="s">
+        <v>237</v>
+      </c>
+      <c r="C27" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" t="s">
+        <v>237</v>
+      </c>
+      <c r="C28" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" t="s">
+        <v>237</v>
+      </c>
+      <c r="C29" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" t="s">
+        <v>237</v>
+      </c>
+      <c r="C30" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" t="s">
+        <v>237</v>
+      </c>
+      <c r="C31" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" t="s">
+        <v>229</v>
+      </c>
+      <c r="C32" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>100</v>
+      </c>
+      <c r="B33" t="s">
+        <v>229</v>
+      </c>
+      <c r="C33" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" t="s">
+        <v>229</v>
+      </c>
+      <c r="C34" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" t="s">
+        <v>229</v>
+      </c>
+      <c r="C35" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
+        <v>229</v>
+      </c>
+      <c r="C36" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" t="s">
+        <v>229</v>
+      </c>
+      <c r="C37" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" t="s">
+        <v>229</v>
+      </c>
+      <c r="C38" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" t="s">
+        <v>229</v>
+      </c>
+      <c r="C39" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" t="s">
+        <v>229</v>
+      </c>
+      <c r="C40" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" t="s">
+        <v>229</v>
+      </c>
+      <c r="C41" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" t="s">
+        <v>229</v>
+      </c>
+      <c r="C42" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" t="s">
+        <v>229</v>
+      </c>
+      <c r="C43" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>104</v>
+      </c>
+      <c r="B44" t="s">
+        <v>229</v>
+      </c>
+      <c r="C44" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>142</v>
+      </c>
+      <c r="B45" t="s">
+        <v>229</v>
+      </c>
+      <c r="C45" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" t="s">
+        <v>227</v>
+      </c>
+      <c r="C46" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47" t="s">
+        <v>225</v>
+      </c>
+      <c r="C47" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" t="s">
+        <v>225</v>
+      </c>
+      <c r="C48" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" t="s">
+        <v>222</v>
+      </c>
+      <c r="C49" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" t="s">
+        <v>222</v>
+      </c>
+      <c r="C50" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" t="s">
+        <v>220</v>
+      </c>
+      <c r="C51" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>104</v>
+      </c>
+      <c r="B52" t="s">
+        <v>218</v>
+      </c>
+      <c r="C52" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" t="s">
+        <v>212</v>
+      </c>
+      <c r="C53" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>97</v>
+      </c>
+      <c r="B54" t="s">
+        <v>212</v>
+      </c>
+      <c r="C54" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>94</v>
+      </c>
+      <c r="B55" t="s">
+        <v>212</v>
+      </c>
+      <c r="C55" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>90</v>
+      </c>
+      <c r="B56" t="s">
+        <v>212</v>
+      </c>
+      <c r="C56" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" t="s">
+        <v>212</v>
+      </c>
+      <c r="C57" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>101</v>
+      </c>
+      <c r="B58" t="s">
+        <v>206</v>
+      </c>
+      <c r="C58" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>100</v>
+      </c>
+      <c r="B59" t="s">
+        <v>206</v>
+      </c>
+      <c r="C59" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>83</v>
+      </c>
+      <c r="B60" t="s">
+        <v>206</v>
+      </c>
+      <c r="C60" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>92</v>
+      </c>
+      <c r="B61" t="s">
+        <v>206</v>
+      </c>
+      <c r="C61" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>86</v>
+      </c>
+      <c r="B62" t="s">
+        <v>206</v>
+      </c>
+      <c r="C62" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>79</v>
+      </c>
+      <c r="B63" t="s">
+        <v>204</v>
+      </c>
+      <c r="C63" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>80</v>
+      </c>
+      <c r="B64" t="s">
+        <v>201</v>
+      </c>
+      <c r="C64" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>79</v>
+      </c>
+      <c r="B65" t="s">
+        <v>201</v>
+      </c>
+      <c r="C65" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>83</v>
+      </c>
+      <c r="B66" t="s">
+        <v>201</v>
+      </c>
+      <c r="C66" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>94</v>
+      </c>
+      <c r="B67" t="s">
+        <v>199</v>
+      </c>
+      <c r="C67" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>94</v>
+      </c>
+      <c r="B68" t="s">
+        <v>197</v>
+      </c>
+      <c r="C68" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>107</v>
+      </c>
+      <c r="B69" t="s">
+        <v>194</v>
+      </c>
+      <c r="C69" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>104</v>
+      </c>
+      <c r="B70" t="s">
+        <v>194</v>
+      </c>
+      <c r="C70" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>107</v>
+      </c>
+      <c r="B71" t="s">
+        <v>192</v>
+      </c>
+      <c r="C71" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>92</v>
+      </c>
+      <c r="B72" t="s">
+        <v>190</v>
+      </c>
+      <c r="C72" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B73" t="s">
+        <v>188</v>
+      </c>
+      <c r="C73" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>100</v>
+      </c>
+      <c r="B74" t="s">
+        <v>186</v>
+      </c>
+      <c r="C74" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>100</v>
+      </c>
+      <c r="B75" t="s">
+        <v>184</v>
+      </c>
+      <c r="C75" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>88</v>
+      </c>
+      <c r="B76" t="s">
+        <v>178</v>
+      </c>
+      <c r="C76" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>107</v>
+      </c>
+      <c r="B77" t="s">
+        <v>178</v>
+      </c>
+      <c r="C77" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>104</v>
+      </c>
+      <c r="B78" t="s">
+        <v>178</v>
+      </c>
+      <c r="C78" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>142</v>
+      </c>
+      <c r="B79" t="s">
+        <v>178</v>
+      </c>
+      <c r="C79" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>156</v>
+      </c>
+      <c r="B80" t="s">
+        <v>178</v>
+      </c>
+      <c r="C80" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>97</v>
+      </c>
+      <c r="B81" t="s">
+        <v>173</v>
+      </c>
+      <c r="C81" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82" t="s">
+        <v>173</v>
+      </c>
+      <c r="C82" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>94</v>
+      </c>
+      <c r="B83" t="s">
+        <v>173</v>
+      </c>
+      <c r="C83" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>90</v>
+      </c>
+      <c r="B84" t="s">
+        <v>173</v>
+      </c>
+      <c r="C84" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>80</v>
+      </c>
+      <c r="B85" t="s">
+        <v>171</v>
+      </c>
+      <c r="C85" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>97</v>
+      </c>
+      <c r="B86" t="s">
+        <v>167</v>
+      </c>
+      <c r="C86" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>83</v>
+      </c>
+      <c r="B87" t="s">
+        <v>167</v>
+      </c>
+      <c r="C87" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>94</v>
+      </c>
+      <c r="B88" t="s">
+        <v>167</v>
+      </c>
+      <c r="C88" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>79</v>
+      </c>
+      <c r="B89" t="s">
+        <v>165</v>
+      </c>
+      <c r="C89" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>101</v>
+      </c>
+      <c r="B90" t="s">
+        <v>155</v>
+      </c>
+      <c r="C90" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>100</v>
+      </c>
+      <c r="B91" t="s">
+        <v>155</v>
+      </c>
+      <c r="C91" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>80</v>
+      </c>
+      <c r="B92" t="s">
+        <v>155</v>
+      </c>
+      <c r="C92" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>79</v>
+      </c>
+      <c r="B93" t="s">
+        <v>155</v>
+      </c>
+      <c r="C93" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>97</v>
+      </c>
+      <c r="B94" t="s">
+        <v>155</v>
+      </c>
+      <c r="C94" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>83</v>
+      </c>
+      <c r="B95" t="s">
+        <v>155</v>
+      </c>
+      <c r="C95" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>155</v>
+      </c>
+      <c r="C96" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>92</v>
+      </c>
+      <c r="B97" t="s">
+        <v>155</v>
+      </c>
+      <c r="C97" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>90</v>
+      </c>
+      <c r="B98" t="s">
+        <v>155</v>
+      </c>
+      <c r="C98" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>88</v>
+      </c>
+      <c r="B99" t="s">
+        <v>155</v>
+      </c>
+      <c r="C99" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>107</v>
+      </c>
+      <c r="B100" t="s">
+        <v>155</v>
+      </c>
+      <c r="C100" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>86</v>
+      </c>
+      <c r="B101" t="s">
+        <v>155</v>
+      </c>
+      <c r="C101" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>104</v>
+      </c>
+      <c r="B102" t="s">
+        <v>155</v>
+      </c>
+      <c r="C102" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>142</v>
+      </c>
+      <c r="B103" t="s">
+        <v>155</v>
+      </c>
+      <c r="C103" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>156</v>
+      </c>
+      <c r="B104" t="s">
+        <v>155</v>
+      </c>
+      <c r="C104" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>101</v>
+      </c>
+      <c r="B105" t="s">
+        <v>141</v>
+      </c>
+      <c r="C105" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>100</v>
+      </c>
+      <c r="B106" t="s">
+        <v>141</v>
+      </c>
+      <c r="C106" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>80</v>
+      </c>
+      <c r="B107" t="s">
+        <v>141</v>
+      </c>
+      <c r="C107" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>79</v>
+      </c>
+      <c r="B108" t="s">
+        <v>141</v>
+      </c>
+      <c r="C108" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>97</v>
+      </c>
+      <c r="B109" t="s">
+        <v>141</v>
+      </c>
+      <c r="C109" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>83</v>
+      </c>
+      <c r="B110" t="s">
+        <v>141</v>
+      </c>
+      <c r="C110" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>94</v>
+      </c>
+      <c r="B111" t="s">
+        <v>141</v>
+      </c>
+      <c r="C111" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>92</v>
+      </c>
+      <c r="B112" t="s">
+        <v>141</v>
+      </c>
+      <c r="C112" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>90</v>
+      </c>
+      <c r="B113" t="s">
+        <v>141</v>
+      </c>
+      <c r="C113" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>88</v>
+      </c>
+      <c r="B114" t="s">
+        <v>141</v>
+      </c>
+      <c r="C114" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>107</v>
+      </c>
+      <c r="B115" t="s">
+        <v>141</v>
+      </c>
+      <c r="C115" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>86</v>
+      </c>
+      <c r="B116" t="s">
+        <v>141</v>
+      </c>
+      <c r="C116" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>104</v>
+      </c>
+      <c r="B117" t="s">
+        <v>141</v>
+      </c>
+      <c r="C117" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>142</v>
+      </c>
+      <c r="B118" t="s">
+        <v>141</v>
+      </c>
+      <c r="C118" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>101</v>
+      </c>
+      <c r="B119" t="s">
+        <v>134</v>
+      </c>
+      <c r="C119" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>100</v>
+      </c>
+      <c r="B120" t="s">
+        <v>134</v>
+      </c>
+      <c r="C120" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>83</v>
+      </c>
+      <c r="B121" t="s">
+        <v>134</v>
+      </c>
+      <c r="C121" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>94</v>
+      </c>
+      <c r="B122" t="s">
+        <v>134</v>
+      </c>
+      <c r="C122" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>92</v>
+      </c>
+      <c r="B123" t="s">
+        <v>134</v>
+      </c>
+      <c r="C123" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>86</v>
+      </c>
+      <c r="B124" t="s">
+        <v>134</v>
+      </c>
+      <c r="C124" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>101</v>
+      </c>
+      <c r="B125" t="s">
+        <v>127</v>
+      </c>
+      <c r="C125" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>100</v>
+      </c>
+      <c r="B126" t="s">
+        <v>127</v>
+      </c>
+      <c r="C126" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>80</v>
+      </c>
+      <c r="B127" t="s">
+        <v>127</v>
+      </c>
+      <c r="C127" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>79</v>
+      </c>
+      <c r="B128" t="s">
+        <v>127</v>
+      </c>
+      <c r="C128" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>83</v>
+      </c>
+      <c r="B129" t="s">
+        <v>127</v>
+      </c>
+      <c r="C129" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>92</v>
+      </c>
+      <c r="B130" t="s">
+        <v>127</v>
+      </c>
+      <c r="C130" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>86</v>
+      </c>
+      <c r="B131" t="s">
+        <v>127</v>
+      </c>
+      <c r="C131" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>104</v>
+      </c>
+      <c r="B132" t="s">
+        <v>125</v>
+      </c>
+      <c r="C132" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>101</v>
+      </c>
+      <c r="B133" t="s">
+        <v>120</v>
+      </c>
+      <c r="C133" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>100</v>
+      </c>
+      <c r="B134" t="s">
+        <v>120</v>
+      </c>
+      <c r="C134" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>83</v>
+      </c>
+      <c r="B135" t="s">
+        <v>120</v>
+      </c>
+      <c r="C135" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>94</v>
+      </c>
+      <c r="B136" t="s">
+        <v>120</v>
+      </c>
+      <c r="C136" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>92</v>
+      </c>
+      <c r="B137" t="s">
+        <v>120</v>
+      </c>
+      <c r="C137" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>86</v>
+      </c>
+      <c r="B138" t="s">
+        <v>120</v>
+      </c>
+      <c r="C138" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>80</v>
+      </c>
+      <c r="B139" t="s">
+        <v>117</v>
+      </c>
+      <c r="C139" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>79</v>
+      </c>
+      <c r="B140" t="s">
+        <v>117</v>
+      </c>
+      <c r="C140" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>80</v>
+      </c>
+      <c r="B141" t="s">
+        <v>115</v>
+      </c>
+      <c r="C141" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>79</v>
+      </c>
+      <c r="B142" t="s">
+        <v>115</v>
+      </c>
+      <c r="C142" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>86</v>
+      </c>
+      <c r="B143" t="s">
+        <v>112</v>
+      </c>
+      <c r="C143" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>104</v>
+      </c>
+      <c r="B144" t="s">
+        <v>112</v>
+      </c>
+      <c r="C144" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>80</v>
+      </c>
+      <c r="B145" t="s">
+        <v>110</v>
+      </c>
+      <c r="C145" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>100</v>
+      </c>
+      <c r="B146" t="s">
+        <v>103</v>
+      </c>
+      <c r="C146" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>107</v>
+      </c>
+      <c r="B147" t="s">
+        <v>103</v>
+      </c>
+      <c r="C147" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>86</v>
+      </c>
+      <c r="B148" t="s">
+        <v>103</v>
+      </c>
+      <c r="C148" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>104</v>
+      </c>
+      <c r="B149" t="s">
+        <v>103</v>
+      </c>
+      <c r="C149" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>101</v>
+      </c>
+      <c r="B150" t="s">
+        <v>85</v>
+      </c>
+      <c r="C150" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>100</v>
+      </c>
+      <c r="B151" t="s">
+        <v>85</v>
+      </c>
+      <c r="C151" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>80</v>
+      </c>
+      <c r="B152" t="s">
+        <v>85</v>
+      </c>
+      <c r="C152" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>79</v>
+      </c>
+      <c r="B153" t="s">
+        <v>85</v>
+      </c>
+      <c r="C153" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>97</v>
+      </c>
+      <c r="B154" t="s">
+        <v>85</v>
+      </c>
+      <c r="C154" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>83</v>
+      </c>
+      <c r="B155" t="s">
+        <v>85</v>
+      </c>
+      <c r="C155" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>94</v>
+      </c>
+      <c r="B156" t="s">
+        <v>85</v>
+      </c>
+      <c r="C156" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>92</v>
+      </c>
+      <c r="B157" t="s">
+        <v>85</v>
+      </c>
+      <c r="C157" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>90</v>
+      </c>
+      <c r="B158" t="s">
+        <v>85</v>
+      </c>
+      <c r="C158" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>88</v>
+      </c>
+      <c r="B159" t="s">
+        <v>85</v>
+      </c>
+      <c r="C159" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>86</v>
+      </c>
+      <c r="B160" t="s">
+        <v>85</v>
+      </c>
+      <c r="C160" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>83</v>
+      </c>
+      <c r="B161" t="s">
+        <v>82</v>
+      </c>
+      <c r="C161" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>80</v>
+      </c>
+      <c r="B162" t="s">
+        <v>78</v>
+      </c>
+      <c r="C162" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>79</v>
+      </c>
+      <c r="B163" t="s">
+        <v>78</v>
+      </c>
+      <c r="C163" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s">
+        <v>307</v>
+      </c>
+      <c r="C5" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" t="s">
+        <v>307</v>
+      </c>
+      <c r="C7" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>314</v>
+      </c>
+      <c r="B8" t="s">
+        <v>307</v>
+      </c>
+      <c r="C8" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>312</v>
+      </c>
+      <c r="B9" t="s">
+        <v>307</v>
+      </c>
+      <c r="C9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" t="s">
+        <v>307</v>
+      </c>
+      <c r="C10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>309</v>
+      </c>
+      <c r="B11" t="s">
+        <v>307</v>
+      </c>
+      <c r="C11" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" t="s">
+        <v>307</v>
+      </c>
+      <c r="C12" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>305</v>
+      </c>
+      <c r="B13" t="s">
+        <v>297</v>
+      </c>
+      <c r="C13" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" t="s">
+        <v>297</v>
+      </c>
+      <c r="C14" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" t="s">
+        <v>297</v>
+      </c>
+      <c r="C15" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>301</v>
+      </c>
+      <c r="B16" t="s">
+        <v>297</v>
+      </c>
+      <c r="C16" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>156</v>
+      </c>
+      <c r="B17" t="s">
+        <v>297</v>
+      </c>
+      <c r="C17" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>298</v>
+      </c>
+      <c r="B18" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>296</v>
+      </c>
+      <c r="B19" t="s">
+        <v>283</v>
+      </c>
+      <c r="C19" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>294</v>
+      </c>
+      <c r="B20" t="s">
+        <v>283</v>
+      </c>
+      <c r="C20" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>292</v>
+      </c>
+      <c r="B21" t="s">
+        <v>283</v>
+      </c>
+      <c r="C21" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>290</v>
+      </c>
+      <c r="B22" t="s">
+        <v>283</v>
+      </c>
+      <c r="C22" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>288</v>
+      </c>
+      <c r="B23" t="s">
+        <v>283</v>
+      </c>
+      <c r="C23" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>286</v>
+      </c>
+      <c r="B24" t="s">
+        <v>283</v>
+      </c>
+      <c r="C24" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>284</v>
+      </c>
+      <c r="B25" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>282</v>
+      </c>
+      <c r="C29" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>280</v>
+      </c>
+      <c r="C30" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>277</v>
+      </c>
+      <c r="C34" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>275</v>
+      </c>
+      <c r="C35" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>273</v>
+      </c>
+      <c r="C36" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>271</v>
+      </c>
+      <c r="C37" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>269</v>
+      </c>
+      <c r="C38" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>267</v>
+      </c>
+      <c r="C39" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>265</v>
+      </c>
+      <c r="C40" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>263</v>
+      </c>
+      <c r="C41" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>261</v>
+      </c>
+      <c r="C42" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>259</v>
+      </c>
+      <c r="C43" t="s">
+        <v>258</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>